<commit_message>
Added runtime results of three more jobs.
git-svn-id: svn+ssh://in.cns.iu.edu/projects/svn/nwb/trunk@4170 c287de05-5010-0410-818a-8f02fb49d6a9
</commit_message>
<xml_diff>
--- a/test-devel/ParallelBatchSOM/run-analysis/ParallelBatchSOM.xlsx
+++ b/test-devel/ParallelBatchSOM/run-analysis/ParallelBatchSOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>dim</t>
   </si>
@@ -92,12 +92,6 @@
   </si>
   <si>
     <t>Big Red run time estimate (m)</t>
-  </si>
-  <si>
-    <t>check earlier run from 12/23</t>
-  </si>
-  <si>
-    <t>check later run from 12/23</t>
   </si>
   <si>
     <t>distance</t>
@@ -193,13 +187,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -236,11 +228,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>(dimensionality</a:t>
+              <a:t>(complexity</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> * #trainingSteps * mapSize / #processes) vs runtime  </a:t>
+              <a:t> guess) vs runtime  </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -270,8 +262,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.37404607757363673"/>
-                  <c:y val="-9.0929036347236827E-2"/>
+                  <c:x val="0.42841722907762575"/>
+                  <c:y val="-8.4308264905997257E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -279,28 +271,37 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$P$6,Sheet1!$P$7,Sheet1!$P$10)</c:f>
+              <c:f>(Sheet1!$P$10,Sheet1!$P$11,Sheet1!$P$12,Sheet1!$P$13,Sheet1!$P$14,Sheet1!$P$15)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>108675000000</c:v>
+                  <c:v>2.1735E+17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1086750000000</c:v>
+                  <c:v>2.1735E+19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>579600000000</c:v>
+                  <c:v>4.6368E+19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1592E+19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.796E+19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.864E+20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$R$6,Sheet1!$R$7,Sheet1!$R$10)</c:f>
+              <c:f>(Sheet1!$R$10,Sheet1!$R$11,Sheet1!$R$12,Sheet1!$R$13,Sheet1!$R$14,Sheet1!$R$15)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -310,27 +311,36 @@
                 <c:pt idx="2">
                   <c:v>51</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>246</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="62916096"/>
-        <c:axId val="62917632"/>
+        <c:axId val="63112704"/>
+        <c:axId val="63114240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62916096"/>
+        <c:axId val="63112704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62917632"/>
+        <c:crossAx val="63114240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62917632"/>
+        <c:axId val="63114240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -338,7 +348,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62916096"/>
+        <c:crossAx val="63112704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -351,7 +361,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -362,15 +372,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -677,15 +687,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
@@ -740,7 +750,7 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
@@ -781,7 +791,7 @@
         <v>10000</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F12" si="0">D2/E2</f>
+        <f t="shared" ref="F2:F3" si="0">D2/E2</f>
         <v>100</v>
       </c>
       <c r="G2">
@@ -791,7 +801,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I12" si="1">G2*H2</f>
+        <f t="shared" ref="I2:I3" si="1">G2*H2</f>
         <v>112</v>
       </c>
       <c r="J2" t="s">
@@ -804,18 +814,18 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N2">
         <v>4</v>
       </c>
       <c r="P2" s="1">
-        <f>B2*D2*I2/N2</f>
-        <v>84000000</v>
+        <f>B2*C2*D2*F2*I2/N2</f>
+        <v>84000000000000</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q12" si="2">0.00000000007*P2 + 7.74</f>
-        <v>7.7458800000000005</v>
+        <f>0.0000000000000000005*P2 + 43.369</f>
+        <v>43.369042</v>
       </c>
       <c r="R2">
         <v>1.3</v>
@@ -861,18 +871,18 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="P3" s="1">
-        <f>B3*D3*I3/N3</f>
-        <v>336000000</v>
+        <f t="shared" ref="P3" si="2">B3*C3*D3*F3*I3/N3</f>
+        <v>336000000000000</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="2"/>
-        <v>7.7635200000000006</v>
+        <f t="shared" ref="Q3" si="3">0.0000000000000000005*P3 + 43.369</f>
+        <v>43.369168000000002</v>
       </c>
       <c r="R3">
         <v>5.2</v>
@@ -880,59 +890,59 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>10000</v>
+        <v>2000000</v>
       </c>
       <c r="D4">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="E4">
         <v>10000</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>D4/E4</f>
+        <v>10</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="H4">
-        <v>14</v>
+        <v>300</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="1"/>
-        <v>112</v>
+        <f>G4*H4</f>
+        <v>75600</v>
       </c>
       <c r="J4" t="s">
         <v>5</v>
       </c>
       <c r="K4">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="L4">
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N4">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1">
-        <f>B4*D4*I4/N4</f>
-        <v>21000000</v>
+        <f>B4*C4*D4*F4*I4/N4</f>
+        <v>4.536E+17</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="2"/>
-        <v>7.7414700000000005</v>
+        <f>0.0000000000000000005*P4 + 43.369</f>
+        <v>43.595799999999997</v>
       </c>
       <c r="R4">
-        <v>0.4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -940,19 +950,19 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2300</v>
       </c>
       <c r="C5">
-        <v>2000000</v>
+        <v>200000</v>
       </c>
       <c r="D5">
-        <v>100000</v>
+        <v>5000</v>
       </c>
       <c r="E5">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
+        <f>D5/E5</f>
         <v>10</v>
       </c>
       <c r="G5">
@@ -962,39 +972,48 @@
         <v>300</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="1"/>
+        <f>G5*H5</f>
         <v>75600</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
       </c>
       <c r="K5">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
       </c>
       <c r="P5" s="1">
-        <f>B5*D5*I5/N5</f>
-        <v>22680000000</v>
+        <f>B5*C5*D5*F5*I5/N5</f>
+        <v>4.347E+17</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="2"/>
-        <v>9.3276000000000003</v>
+        <f>0.0000000000000000005*P5 + 43.369</f>
+        <v>43.586350000000003</v>
       </c>
       <c r="R5">
-        <v>60</v>
+        <v>6.5</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>2300</v>
@@ -1003,14 +1022,14 @@
         <v>200000</v>
       </c>
       <c r="D6">
-        <v>5000</v>
+        <v>50000</v>
       </c>
       <c r="E6">
         <v>500</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>D6/E6</f>
+        <v>100</v>
       </c>
       <c r="G6">
         <v>252</v>
@@ -1019,7 +1038,7 @@
         <v>300</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="1"/>
+        <f>G6*H6</f>
         <v>75600</v>
       </c>
       <c r="J6" t="s">
@@ -1032,213 +1051,84 @@
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P6" s="1">
-        <f>B6*D6*I6/N6</f>
-        <v>108675000000</v>
+        <f>B6*C6*D6*F6*I6/N6</f>
+        <v>4.347E+19</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="2"/>
-        <v>15.347250000000001</v>
+        <f>0.0000000000000000005*P6 + 43.369</f>
+        <v>65.103999999999999</v>
       </c>
       <c r="R6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>2300</v>
-      </c>
-      <c r="C7">
-        <v>200000</v>
-      </c>
-      <c r="D7">
-        <v>50000</v>
-      </c>
-      <c r="E7">
-        <v>500</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G7">
-        <v>252</v>
-      </c>
-      <c r="H7">
-        <v>300</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="1"/>
-        <v>75600</v>
-      </c>
-      <c r="J7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7">
-        <v>250</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7">
-        <v>8</v>
-      </c>
-      <c r="O7">
-        <v>2</v>
-      </c>
-      <c r="P7" s="1">
-        <f>B7*D7*I7/N7</f>
-        <v>1086750000000</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="2"/>
-        <v>83.8125</v>
-      </c>
-      <c r="R7">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>2300</v>
-      </c>
-      <c r="C8">
-        <v>200000</v>
-      </c>
-      <c r="D8">
-        <v>5000</v>
-      </c>
-      <c r="E8">
-        <v>500</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>252</v>
-      </c>
-      <c r="H8">
-        <v>300</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="1"/>
-        <v>75600</v>
-      </c>
-      <c r="J8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8">
-        <v>250</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8">
-        <v>4</v>
-      </c>
-      <c r="O8">
-        <v>4</v>
-      </c>
-      <c r="P8" s="1">
-        <f>B8*D8*I8/N8</f>
-        <v>217350000000</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="2"/>
-        <v>22.954500000000003</v>
-      </c>
-      <c r="R8">
-        <v>6.5</v>
-      </c>
-      <c r="S8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="T8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>2300</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>200000</v>
+        <v>10000</v>
       </c>
       <c r="D9">
-        <v>50000</v>
+        <v>1000000</v>
       </c>
       <c r="E9">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
+        <f>D9/E9</f>
         <v>100</v>
       </c>
       <c r="G9">
-        <v>252</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>300</v>
+        <v>14</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="1"/>
-        <v>75600</v>
+        <f>G9*H9</f>
+        <v>112</v>
       </c>
       <c r="J9" t="s">
         <v>5</v>
       </c>
       <c r="K9">
-        <v>250</v>
+        <v>8</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="P9" s="1">
-        <f>B9*D9*I9/N9</f>
-        <v>2173500000000</v>
+        <f>B9*C9*D9*F9*I9/N9</f>
+        <v>21000000000000</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="2"/>
-        <v>159.88500000000002</v>
+        <f>0.0000000000000000005*P9 + 43.369</f>
+        <v>43.369010500000002</v>
       </c>
       <c r="R9">
-        <v>44</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>19</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1252,14 +1142,14 @@
         <v>200000</v>
       </c>
       <c r="D10">
-        <v>200000</v>
+        <v>5000</v>
       </c>
       <c r="E10">
         <v>500</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>400</v>
+        <f>D10/E10</f>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>252</v>
@@ -1268,7 +1158,7 @@
         <v>300</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="1"/>
+        <f>G10*H10</f>
         <v>75600</v>
       </c>
       <c r="J10" t="s">
@@ -1281,27 +1171,24 @@
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N10">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="O10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P10" s="1">
-        <f>B10*D10*I10/N10</f>
-        <v>579600000000</v>
+        <f>B10*C10*D10*F10*I10/N10</f>
+        <v>2.1735E+17</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="2"/>
-        <v>48.312000000000005</v>
+        <f>0.0000000000000000005*P10 + 43.369</f>
+        <v>43.477674999999998</v>
       </c>
       <c r="R10">
-        <v>51</v>
-      </c>
-      <c r="T10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1315,14 +1202,14 @@
         <v>200000</v>
       </c>
       <c r="D11">
-        <v>500000</v>
+        <v>50000</v>
       </c>
       <c r="E11">
-        <v>1000</v>
-      </c>
-      <c r="F11" s="6">
-        <f t="shared" si="0"/>
         <v>500</v>
+      </c>
+      <c r="F11" s="1">
+        <f>D11/E11</f>
+        <v>100</v>
       </c>
       <c r="G11">
         <v>252</v>
@@ -1330,8 +1217,8 @@
       <c r="H11">
         <v>300</v>
       </c>
-      <c r="I11" s="6">
-        <f t="shared" si="1"/>
+      <c r="I11" s="1">
+        <f>G11*H11</f>
         <v>75600</v>
       </c>
       <c r="J11" t="s">
@@ -1344,24 +1231,24 @@
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N11">
-        <v>150</v>
+        <v>8</v>
       </c>
       <c r="O11">
-        <v>3</v>
-      </c>
-      <c r="P11" s="6">
-        <f>B11*D11*I11/N11</f>
-        <v>579600000000</v>
+        <v>2</v>
+      </c>
+      <c r="P11" s="1">
+        <f>B11*C11*D11*F11*I11/N11</f>
+        <v>2.1735E+19</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="2"/>
-        <v>48.312000000000005</v>
-      </c>
-      <c r="R11" t="s">
-        <v>26</v>
+        <f>0.0000000000000000005*P11 + 43.369</f>
+        <v>54.236499999999999</v>
+      </c>
+      <c r="R11">
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1372,17 +1259,17 @@
         <v>2300</v>
       </c>
       <c r="C12">
-        <v>2000000</v>
+        <v>200000</v>
       </c>
       <c r="D12">
-        <v>500000</v>
+        <v>200000</v>
       </c>
       <c r="E12">
-        <v>1000</v>
-      </c>
-      <c r="F12" s="6">
-        <f t="shared" si="0"/>
         <v>500</v>
+      </c>
+      <c r="F12" s="1">
+        <f>D12/E12</f>
+        <v>400</v>
       </c>
       <c r="G12">
         <v>252</v>
@@ -1390,8 +1277,8 @@
       <c r="H12">
         <v>300</v>
       </c>
-      <c r="I12" s="6">
-        <f t="shared" si="1"/>
+      <c r="I12" s="1">
+        <f>G12*H12</f>
         <v>75600</v>
       </c>
       <c r="J12" t="s">
@@ -1404,156 +1291,261 @@
         <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N12">
-        <v>225</v>
+        <v>60</v>
       </c>
       <c r="O12">
         <v>3</v>
       </c>
-      <c r="P12" s="6">
-        <f>B12*D12*I12/N12</f>
-        <v>386400000000</v>
+      <c r="P12" s="1">
+        <f>B12*C12*D12*F12*I12/N12</f>
+        <v>4.6368E+19</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="2"/>
-        <v>34.788000000000004</v>
-      </c>
-      <c r="R12" t="s">
+        <f>0.0000000000000000005*P12 + 43.369</f>
+        <v>66.552999999999997</v>
+      </c>
+      <c r="R12">
+        <v>51</v>
+      </c>
+      <c r="T12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>2300</v>
+      </c>
+      <c r="C13">
+        <v>200000</v>
+      </c>
+      <c r="D13">
+        <v>200000</v>
+      </c>
+      <c r="E13">
+        <v>2000</v>
+      </c>
+      <c r="F13" s="4">
+        <f>D13/E13</f>
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>252</v>
+      </c>
+      <c r="H13">
+        <v>300</v>
+      </c>
+      <c r="I13" s="4">
+        <f>G13*H13</f>
+        <v>75600</v>
+      </c>
+      <c r="J13" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13">
+        <v>250</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
         <v>27</v>
+      </c>
+      <c r="N13">
+        <v>60</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13" s="1">
+        <f>B13*C13*D13*F13*I13/N13</f>
+        <v>1.1592E+19</v>
+      </c>
+      <c r="Q13">
+        <f>0.0000000000000000005*P13 + 43.369</f>
+        <v>49.164999999999999</v>
+      </c>
+      <c r="R13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>2300</v>
+      </c>
+      <c r="C14">
+        <v>200000</v>
+      </c>
+      <c r="D14">
+        <v>500000</v>
+      </c>
+      <c r="E14">
+        <v>1000</v>
+      </c>
+      <c r="F14" s="4">
+        <f>D14/E14</f>
+        <v>500</v>
+      </c>
+      <c r="G14">
+        <v>252</v>
+      </c>
+      <c r="H14">
+        <v>300</v>
+      </c>
+      <c r="I14" s="4">
+        <f>G14*H14</f>
+        <v>75600</v>
+      </c>
+      <c r="J14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>250</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14">
+        <v>150</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14" s="1">
+        <f>B14*C14*D14*F14*I14/N14</f>
+        <v>5.796E+19</v>
+      </c>
+      <c r="Q14">
+        <f>0.0000000000000000005*P14 + 43.369</f>
+        <v>72.349000000000004</v>
+      </c>
+      <c r="R14">
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
         <v>2300</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
+      <c r="C15">
         <v>2000000</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3">
+      <c r="D15">
+        <v>500000</v>
+      </c>
+      <c r="E15">
+        <v>1000</v>
+      </c>
+      <c r="F15" s="4">
+        <f>D15/E15</f>
+        <v>500</v>
+      </c>
+      <c r="G15">
         <v>252</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15">
         <v>300</v>
       </c>
       <c r="I15" s="4">
         <f>G15*H15</f>
         <v>75600</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="N15" s="3">
-        <v>60</v>
-      </c>
-      <c r="O15" s="3"/>
-      <c r="P15" s="5">
-        <f>B15*D15*I15/N15</f>
-        <v>5796000000000</v>
-      </c>
-      <c r="Q15" s="3">
-        <f>0.00000000007*P15 + 7.74</f>
-        <v>413.46000000000004</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
+      <c r="J15" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>250</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15">
+        <v>225</v>
+      </c>
+      <c r="O15">
+        <v>3</v>
+      </c>
+      <c r="P15" s="1">
+        <f>B15*C15*D15*F15*I15/N15</f>
+        <v>3.864E+20</v>
+      </c>
+      <c r="Q15">
+        <f>0.0000000000000000005*P15 + 43.369</f>
+        <v>236.56900000000002</v>
+      </c>
+      <c r="R15">
+        <v>246</v>
+      </c>
     </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3">
+    <row r="18" spans="1:20">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3">
         <v>2300</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3">
+      <c r="C18" s="3">
+        <v>2000000</v>
+      </c>
+      <c r="D18" s="3">
         <f>2000000*50</f>
         <v>100000000</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3">
+      <c r="E18" s="3">
+        <v>50000</v>
+      </c>
+      <c r="F18" s="4">
+        <f>D18/E18</f>
+        <v>2000</v>
+      </c>
+      <c r="G18" s="3">
         <v>252</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H18" s="3">
         <v>300</v>
       </c>
-      <c r="I16" s="4">
-        <f>G16*H16</f>
+      <c r="I18" s="4">
+        <f>G18*H18</f>
         <v>75600</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="N16" s="3">
-        <v>60</v>
-      </c>
-      <c r="O16" s="3"/>
-      <c r="P16" s="5">
-        <f>B16*D16*I16/N16</f>
-        <v>289800000000000</v>
-      </c>
-      <c r="Q16" s="3">
-        <f>0.00000000007*P16 + 7.74</f>
-        <v>20293.740000000002</v>
-      </c>
-      <c r="R16" s="3" t="s">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="N18" s="3">
+        <f>O18*100</f>
+        <v>300</v>
+      </c>
+      <c r="O18" s="3">
+        <v>3</v>
+      </c>
+      <c r="P18" s="1">
+        <f>B18*C18*D18*F18*I18/N18</f>
+        <v>2.3183999999999999E+23</v>
+      </c>
+      <c r="Q18">
+        <f>0.0000000000000000005*P18 + 43.369</f>
+        <v>115963.36900000001</v>
+      </c>
+      <c r="R18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3">
-        <v>2300</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3">
-        <f>2000000*50</f>
-        <v>100000000</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3">
-        <v>252</v>
-      </c>
-      <c r="H17" s="3">
-        <v>300</v>
-      </c>
-      <c r="I17" s="4">
-        <f>G17*H17</f>
-        <v>75600</v>
-      </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="N17" s="3">
-        <f>O17*100</f>
-        <v>300</v>
-      </c>
-      <c r="O17" s="3">
-        <v>3</v>
-      </c>
-      <c r="P17" s="5">
-        <f>B17*D17*I17/N17</f>
-        <v>57960000000000</v>
-      </c>
-      <c r="Q17" s="3">
-        <f>0.00000000007*P17 + 7.74</f>
-        <v>4064.94</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:S10">

</xml_diff>